<commit_message>
add page scope for watch number of registration
</commit_message>
<xml_diff>
--- a/userregistronevent.xlsx
+++ b/userregistronevent.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -67,28 +67,7 @@
     <t>аудитория</t>
   </si>
   <si>
-    <t>Суханов</t>
-  </si>
-  <si>
-    <t>Игорь</t>
-  </si>
-  <si>
-    <t>Константинович</t>
-  </si>
-  <si>
-    <t>you@me.they</t>
-  </si>
-  <si>
-    <t>456542145</t>
-  </si>
-  <si>
-    <t>21.11.2001</t>
-  </si>
-  <si>
-    <t>штаб</t>
-  </si>
-  <si>
-    <t>2019-08-03 00:00:00</t>
+    <t>2019-09-18 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -420,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -485,34 +464,8 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>